<commit_message>
Finished last experimental trials pre-presentation
</commit_message>
<xml_diff>
--- a/doc/data/brave-new-world-trial-data.xlsx
+++ b/doc/data/brave-new-world-trial-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="21">
   <si>
     <t>Conditions:</t>
   </si>
@@ -73,13 +73,19 @@
   </si>
   <si>
     <t>T_Avg</t>
+  </si>
+  <si>
+    <t>Location Memory</t>
+  </si>
+  <si>
+    <t>T_SD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +113,13 @@
       <b/>
       <sz val="11"/>
       <color theme="3" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,13 +157,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,72 +459,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="R1" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
@@ -523,9 +544,49 @@
       <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="5"/>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
+      <c r="K2">
+        <v>12</v>
+      </c>
+      <c r="L2">
+        <v>8</v>
+      </c>
+      <c r="M2">
+        <v>9</v>
+      </c>
+      <c r="N2">
+        <v>9</v>
+      </c>
+      <c r="O2">
+        <v>10</v>
+      </c>
+      <c r="P2">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="5">
+        <f t="shared" ref="Q2" si="0">SUM(G2:P2)/10</f>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="R2" s="6">
+        <f>STDEV(G2:P2)</f>
+        <v>2.0439612955674531</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
@@ -538,9 +599,49 @@
       <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="5"/>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+      <c r="I3">
+        <v>13</v>
+      </c>
+      <c r="J3">
+        <v>12</v>
+      </c>
+      <c r="K3">
+        <v>13</v>
+      </c>
+      <c r="L3">
+        <v>9</v>
+      </c>
+      <c r="M3">
+        <v>14</v>
+      </c>
+      <c r="N3">
+        <v>14</v>
+      </c>
+      <c r="O3">
+        <v>12</v>
+      </c>
+      <c r="P3">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="5">
+        <f>SUM(G3:P3)/10</f>
+        <v>11.5</v>
+      </c>
+      <c r="R3" s="6">
+        <f t="shared" ref="R3:R11" si="1">STDEV(G3:P3)</f>
+        <v>2.5055493963954847</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
@@ -553,14 +654,24 @@
       <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="5"/>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="5">
+        <f>SUM(G4:P4)/10</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
+      <c r="C5" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>16</v>
@@ -568,29 +679,49 @@
       <c r="E5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P5" s="5"/>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q5" s="5">
+        <f>SUM(G5:P5)/10</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="6" t="e">
+        <f>STDEV(G5:P5)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="P6" s="5"/>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q6" s="5">
+        <f>SUM(G6:P6)/10</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="6" t="e">
+        <f>STDEV(G6:P6)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
+      <c r="C7" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>16</v>
@@ -598,75 +729,134 @@
       <c r="E7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P7" s="5"/>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="F7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q7" s="5">
+        <f>SUM(G7:P7)/10</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>16</v>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P8" s="5"/>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="P9" s="5"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="1" t="s">
+      <c r="F8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q8" s="5">
+        <f>SUM(G8:P8)/10</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q9" s="5">
+        <f>SUM(G9:P9)/10</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="Q10" s="5">
+        <f>SUM(G10:P10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="R10" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10">
-        <v>10</v>
-      </c>
-      <c r="G10">
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>7</v>
+      </c>
+      <c r="J11">
+        <v>8</v>
+      </c>
+      <c r="K11">
+        <v>5</v>
+      </c>
+      <c r="L11">
         <v>9</v>
       </c>
-      <c r="H10">
-        <v>6</v>
-      </c>
-      <c r="I10">
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <v>8</v>
+      </c>
+      <c r="O11">
         <v>7</v>
       </c>
-      <c r="J10">
-        <v>5</v>
-      </c>
-      <c r="K10">
-        <v>7</v>
-      </c>
-      <c r="L10">
-        <v>10</v>
-      </c>
-      <c r="M10">
-        <v>6</v>
-      </c>
-      <c r="N10">
-        <v>7</v>
-      </c>
-      <c r="O10">
-        <v>4</v>
-      </c>
-      <c r="P10" s="5">
-        <f>SUM(F10:O10)/10</f>
-        <v>7.1</v>
+      <c r="P11">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="5">
+        <f>SUM(G11:P11)/10</f>
+        <v>5.9</v>
+      </c>
+      <c r="R11" s="6">
+        <f t="shared" si="1"/>
+        <v>2.2827858224351902</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Intermediary commit working on autonomous condition
</commit_message>
<xml_diff>
--- a/doc/data/brave-new-world-trial-data.xlsx
+++ b/doc/data/brave-new-world-trial-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>T1</t>
   </si>
@@ -493,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -510,7 +510,7 @@
     <col min="8" max="8" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -556,8 +556,9 @@
       <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" s="6"/>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -605,8 +606,9 @@
         <f>STDEV(D2:M2)</f>
         <v>2.2827858224351902</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="P2" s="6"/>
+    </row>
+    <row r="3" spans="1:16">
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
@@ -651,8 +653,9 @@
         <f>STDEV(D3:M3)</f>
         <v>2.0439612955674531</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="P3" s="6"/>
+    </row>
+    <row r="4" spans="1:16">
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -697,8 +700,9 @@
         <f t="shared" ref="O4" si="2">STDEV(D4:M4)</f>
         <v>2.5055493963954847</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="P4" s="6"/>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -724,7 +728,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7" s="7" t="s">
         <v>26</v>
       </c>
@@ -736,7 +740,7 @@
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16">
       <c r="A8" s="8" t="s">
         <v>0</v>
       </c>
@@ -762,7 +766,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:16">
       <c r="A9" s="8" t="s">
         <v>1</v>
       </c>
@@ -788,7 +792,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16">
       <c r="A10" s="8" t="s">
         <v>2</v>
       </c>
@@ -814,7 +818,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:16">
       <c r="A11" s="8" t="s">
         <v>3</v>
       </c>
@@ -840,7 +844,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16">
       <c r="A12" s="8" t="s">
         <v>4</v>
       </c>
@@ -866,7 +870,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16">
       <c r="A13" s="8" t="s">
         <v>5</v>
       </c>
@@ -892,7 +896,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:16">
       <c r="A14" s="8" t="s">
         <v>6</v>
       </c>
@@ -916,6 +920,84 @@
       </c>
       <c r="H14" s="8">
         <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="8">
+        <v>700</v>
+      </c>
+      <c r="C15" s="8">
+        <v>12</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H15" s="8">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="8">
+        <v>660</v>
+      </c>
+      <c r="C16" s="8">
+        <v>14</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0.47</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0.26</v>
+      </c>
+      <c r="H16" s="8">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="8">
+        <v>760</v>
+      </c>
+      <c r="C17" s="8">
+        <v>18</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.42</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0.17</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.21</v>
+      </c>
+      <c r="G17" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="H17" s="8">
+        <v>0.28999999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweaked loading screen info
</commit_message>
<xml_diff>
--- a/doc/data/brave-new-world-trial-data.xlsx
+++ b/doc/data/brave-new-world-trial-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>T1</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Baseline Control (random tools)</t>
+  </si>
+  <si>
+    <t>Autonomous Bot (self-deciding)</t>
   </si>
 </sst>
 </file>
@@ -143,7 +146,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,6 +171,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -181,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -191,6 +200,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -998,6 +1009,75 @@
       </c>
       <c r="H17" s="8">
         <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="10">
+        <v>720</v>
+      </c>
+      <c r="C19" s="10">
+        <v>13</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0.47</v>
+      </c>
+      <c r="F19" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="G19" s="10">
+        <v>0.45</v>
+      </c>
+      <c r="H19" s="10">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="10">
+        <v>920</v>
+      </c>
+      <c r="C20" s="10">
+        <v>13</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0.71</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0.22</v>
+      </c>
+      <c r="F20" s="10">
+        <v>0.16</v>
+      </c>
+      <c r="G20" s="10">
+        <v>0.45</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished running experiment trials in excel doc
</commit_message>
<xml_diff>
--- a/doc/data/brave-new-world-trial-data.xlsx
+++ b/doc/data/brave-new-world-trial-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>T1</t>
   </si>
@@ -504,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1076,8 +1076,211 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" t="s">
+      <c r="A21" s="10" t="s">
         <v>2</v>
+      </c>
+      <c r="B21" s="10">
+        <v>930</v>
+      </c>
+      <c r="C21" s="10">
+        <v>10</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0.93</v>
+      </c>
+      <c r="E21" s="10">
+        <v>0.38</v>
+      </c>
+      <c r="F21" s="10">
+        <v>0.16</v>
+      </c>
+      <c r="G21" s="10">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H21" s="10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="10">
+        <v>1000</v>
+      </c>
+      <c r="C22" s="10">
+        <v>21</v>
+      </c>
+      <c r="D22" s="10">
+        <v>0.48</v>
+      </c>
+      <c r="E22" s="10">
+        <v>0.37</v>
+      </c>
+      <c r="F22" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="G22" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H22" s="10">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="10">
+        <v>1200</v>
+      </c>
+      <c r="C23" s="10">
+        <v>23</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0.52</v>
+      </c>
+      <c r="E23" s="10">
+        <v>0.48</v>
+      </c>
+      <c r="F23" s="10">
+        <v>0.27</v>
+      </c>
+      <c r="G23" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="H23" s="10">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="10">
+        <v>720</v>
+      </c>
+      <c r="C24" s="10">
+        <v>10</v>
+      </c>
+      <c r="D24" s="10">
+        <v>0.72</v>
+      </c>
+      <c r="E24" s="10">
+        <v>0.33</v>
+      </c>
+      <c r="F24" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="G24" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H24" s="10">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="10">
+        <v>690</v>
+      </c>
+      <c r="C25" s="10">
+        <v>8</v>
+      </c>
+      <c r="D25" s="10">
+        <v>0.86</v>
+      </c>
+      <c r="E25" s="10">
+        <v>0.36</v>
+      </c>
+      <c r="F25" s="10">
+        <v>0.16</v>
+      </c>
+      <c r="G25" s="10">
+        <v>0.32</v>
+      </c>
+      <c r="H25" s="10">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="10">
+        <v>1130</v>
+      </c>
+      <c r="C26" s="10">
+        <v>17</v>
+      </c>
+      <c r="D26" s="10">
+        <v>0.66</v>
+      </c>
+      <c r="E26" s="10">
+        <v>0.35</v>
+      </c>
+      <c r="F26" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="G26" s="10">
+        <v>0.33</v>
+      </c>
+      <c r="H26" s="10">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="10">
+        <v>1060</v>
+      </c>
+      <c r="C27" s="10">
+        <v>11</v>
+      </c>
+      <c r="D27" s="10">
+        <v>0.96</v>
+      </c>
+      <c r="E27" s="10">
+        <v>0.42</v>
+      </c>
+      <c r="F27" s="10">
+        <v>0.22</v>
+      </c>
+      <c r="G27" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="H27" s="10">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="10">
+        <v>700</v>
+      </c>
+      <c r="C28" s="10">
+        <v>12</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E28" s="10">
+        <v>0.35</v>
+      </c>
+      <c r="F28" s="10">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G28" s="10">
+        <v>0.49</v>
+      </c>
+      <c r="H28" s="10">
+        <v>0.19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>